<commit_message>
converter main part is done
</commit_message>
<xml_diff>
--- a/sources/Course Memo_Spring 2023_ver05_10.01.23_updated by Serik M.xlsx
+++ b/sources/Course Memo_Spring 2023_ver05_10.01.23_updated by Serik M.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UCA-schedule-generator\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\oneku16\learnings\UCA-schedule-generator\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBCE454-04E9-478E-BF71-02A53210CBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE075A5-E9C6-4410-9A94-85F10F1FD1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2966C313-9ED0-4D1C-A2BE-A20E4734B1E8}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{2966C313-9ED0-4D1C-A2BE-A20E4734B1E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 2023" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="134">
   <si>
     <t>Course Code</t>
   </si>
@@ -213,15 +213,6 @@
     <t>Programming II</t>
   </si>
   <si>
-    <t>Database Management Systems </t>
-  </si>
-  <si>
-    <t>Digital Logic &amp; Design </t>
-  </si>
-  <si>
-    <t>Data Structure and Algorithms   </t>
-  </si>
-  <si>
     <t>Statistics II</t>
   </si>
   <si>
@@ -436,6 +427,18 @@
   </si>
   <si>
     <t>training session</t>
+  </si>
+  <si>
+    <t>Data Structure and Algorithms</t>
+  </si>
+  <si>
+    <t>Database Management Systems</t>
+  </si>
+  <si>
+    <t>Digital Logic &amp; Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Academic Writing: Research, Fiction and Nonfiction    </t>
   </si>
 </sst>
 </file>
@@ -793,7 +796,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -809,9 +812,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -849,7 +852,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -955,7 +958,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1108,10 +1111,10 @@
   <dimension ref="A1:U62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L57" sqref="L57"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1208,7 @@
         <v>9002</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>10</v>
@@ -1233,10 +1236,10 @@
         <v>13</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O3" s="16"/>
     </row>
@@ -1276,10 +1279,10 @@
         <v>13</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O4" s="16"/>
     </row>
@@ -1319,7 +1322,7 @@
         <v>25</v>
       </c>
       <c r="M5" s="30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="N5" s="30"/>
       <c r="O5" s="51"/>
@@ -1360,7 +1363,7 @@
         <v>25</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="N6" s="30"/>
       <c r="O6" s="51"/>
@@ -1401,7 +1404,7 @@
         <v>26</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N7" s="12"/>
       <c r="O7" s="16"/>
@@ -1442,7 +1445,7 @@
         <v>26</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N8" s="12"/>
       <c r="O8" s="16"/>
@@ -1474,7 +1477,7 @@
         <v>1002</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>10</v>
@@ -1500,7 +1503,7 @@
         <v>27</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N10" s="11"/>
       <c r="O10" s="5"/>
@@ -1539,7 +1542,7 @@
         <v>27</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N11" s="12"/>
       <c r="O11" s="16"/>
@@ -1578,7 +1581,7 @@
         <v>27</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N12" s="12"/>
       <c r="O12" s="16"/>
@@ -1617,7 +1620,7 @@
         <v>14</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N13" s="22"/>
       <c r="O13" s="21"/>
@@ -1656,7 +1659,7 @@
         <v>14</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
@@ -1695,7 +1698,7 @@
         <v>14</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N15" s="22"/>
       <c r="O15" s="22"/>
@@ -1734,7 +1737,7 @@
         <v>14</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N16" s="12"/>
       <c r="O16" s="16"/>
@@ -1764,7 +1767,7 @@
       </c>
       <c r="I17" s="23"/>
       <c r="J17" s="18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K17" s="17">
         <v>16</v>
@@ -1773,7 +1776,7 @@
         <v>36</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N17" s="12"/>
       <c r="O17" s="16"/>
@@ -1786,7 +1789,7 @@
         <v>3082</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>58</v>
+        <v>131</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>10</v>
@@ -1812,7 +1815,7 @@
         <v>14</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N18" s="12"/>
       <c r="O18" s="5"/>
@@ -1825,7 +1828,7 @@
         <v>2021</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>10</v>
@@ -1851,7 +1854,7 @@
         <v>27</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N19" s="12"/>
       <c r="O19" s="5"/>
@@ -1864,7 +1867,7 @@
         <v>2041</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>10</v>
@@ -1890,7 +1893,7 @@
         <v>27</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N20" s="12"/>
       <c r="O20" s="5"/>
@@ -1908,7 +1911,7 @@
         <v>2011</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>31</v>
@@ -1934,7 +1937,7 @@
         <v>27</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N21" s="12"/>
       <c r="O21" s="5"/>
@@ -1947,7 +1950,7 @@
         <v>1003</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>10</v>
@@ -1973,7 +1976,7 @@
         <v>33</v>
       </c>
       <c r="M22" s="22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N22" s="18"/>
       <c r="O22" s="37"/>
@@ -2011,10 +2014,10 @@
       <c r="J23" s="11"/>
       <c r="K23" s="17"/>
       <c r="L23" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N23" s="11"/>
       <c r="O23" s="5"/>
@@ -2044,7 +2047,7 @@
       </c>
       <c r="I24" s="17"/>
       <c r="J24" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K24" s="17">
         <v>16</v>
@@ -2053,7 +2056,7 @@
         <v>36</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N24" s="11"/>
       <c r="O24" s="5"/>
@@ -2066,7 +2069,7 @@
         <v>3023</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>10</v>
@@ -2092,7 +2095,7 @@
         <v>14</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N25" s="11"/>
       <c r="O25" s="5"/>
@@ -2102,10 +2105,10 @@
         <v>55</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>31</v>
@@ -2131,7 +2134,7 @@
         <v>27</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N26" s="11"/>
       <c r="O26" s="11"/>
@@ -2141,10 +2144,10 @@
         <v>52</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>31</v>
@@ -2161,7 +2164,7 @@
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K27" s="17">
         <v>16</v>
@@ -2170,7 +2173,7 @@
         <v>27</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="N27" s="11"/>
       <c r="O27" s="5"/>
@@ -2183,7 +2186,7 @@
         <v>3052</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>10</v>
@@ -2209,7 +2212,7 @@
         <v>27</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N28" s="11"/>
       <c r="O28" s="5"/>
@@ -2224,10 +2227,10 @@
         <v>50</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>31</v>
@@ -2253,7 +2256,7 @@
         <v>14</v>
       </c>
       <c r="M29" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N29" s="32"/>
       <c r="O29" s="32"/>
@@ -2266,7 +2269,7 @@
         <v>4071</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>10</v>
@@ -2292,7 +2295,7 @@
         <v>14</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N30" s="11"/>
       <c r="O30" s="5"/>
@@ -2322,7 +2325,7 @@
       </c>
       <c r="I31" s="17"/>
       <c r="J31" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K31" s="17">
         <v>16</v>
@@ -2331,7 +2334,7 @@
         <v>36</v>
       </c>
       <c r="M31" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N31" s="11"/>
       <c r="O31" s="5"/>
@@ -2350,7 +2353,7 @@
         <v>4011</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>10</v>
@@ -2376,7 +2379,7 @@
         <v>14</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N32" s="11"/>
       <c r="O32" s="5"/>
@@ -2386,10 +2389,10 @@
         <v>50</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>31</v>
@@ -2415,7 +2418,7 @@
         <v>27</v>
       </c>
       <c r="M33" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N33" s="11"/>
       <c r="O33" s="5"/>
@@ -2425,10 +2428,10 @@
         <v>50</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>31</v>
@@ -2454,7 +2457,7 @@
         <v>27</v>
       </c>
       <c r="M34" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N34" s="11"/>
       <c r="O34" s="5"/>
@@ -2464,10 +2467,10 @@
         <v>50</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>31</v>
@@ -2493,7 +2496,7 @@
         <v>27</v>
       </c>
       <c r="M35" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N35" s="32"/>
       <c r="O35" s="32"/>
@@ -2506,7 +2509,7 @@
         <v>4812</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>10</v>
@@ -2532,7 +2535,7 @@
         <v>14</v>
       </c>
       <c r="M36" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N36" s="11"/>
       <c r="O36" s="11"/>
@@ -2564,7 +2567,7 @@
         <v>1002</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>10</v>
@@ -2590,7 +2593,7 @@
         <v>27</v>
       </c>
       <c r="M38" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N38" s="11"/>
       <c r="O38" s="5"/>
@@ -2603,7 +2606,7 @@
         <v>1211</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>10</v>
@@ -2629,7 +2632,7 @@
         <v>14</v>
       </c>
       <c r="M39" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N39" s="12"/>
       <c r="O39" s="16"/>
@@ -2668,7 +2671,7 @@
         <v>14</v>
       </c>
       <c r="M40" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N40" s="12"/>
       <c r="O40" s="16"/>
@@ -2707,7 +2710,7 @@
         <v>14</v>
       </c>
       <c r="M41" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N41" s="12"/>
       <c r="O41" s="12"/>
@@ -2746,7 +2749,7 @@
         <v>14</v>
       </c>
       <c r="M42" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N42" s="12"/>
       <c r="O42" s="12"/>
@@ -2785,7 +2788,7 @@
         <v>14</v>
       </c>
       <c r="M43" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N43" s="12"/>
       <c r="O43" s="16"/>
@@ -2798,7 +2801,7 @@
         <v>1070</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D44" s="13" t="s">
         <v>10</v>
@@ -2824,7 +2827,7 @@
         <v>14</v>
       </c>
       <c r="M44" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N44" s="12"/>
       <c r="O44" s="5"/>
@@ -2854,7 +2857,7 @@
       </c>
       <c r="I45" s="17"/>
       <c r="J45" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K45" s="17">
         <v>16</v>
@@ -2863,7 +2866,7 @@
         <v>36</v>
       </c>
       <c r="M45" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N45" s="12"/>
       <c r="O45" s="5"/>
@@ -2902,7 +2905,7 @@
         <v>14</v>
       </c>
       <c r="M46" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N46" s="34"/>
       <c r="O46" s="34"/>
@@ -2915,7 +2918,7 @@
         <v>1002</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D47" s="13" t="s">
         <v>10</v>
@@ -2941,7 +2944,7 @@
         <v>27</v>
       </c>
       <c r="M47" s="12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N47" s="12"/>
       <c r="O47" s="16"/>
@@ -2954,7 +2957,7 @@
         <v>2031</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D48" s="13" t="s">
         <v>10</v>
@@ -2980,7 +2983,7 @@
         <v>27</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N48" s="11"/>
       <c r="O48" s="5"/>
@@ -2993,7 +2996,7 @@
         <v>2164</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D49" s="13" t="s">
         <v>10</v>
@@ -3019,7 +3022,7 @@
         <v>14</v>
       </c>
       <c r="M49" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N49" s="11"/>
       <c r="O49" s="5"/>
@@ -3032,7 +3035,7 @@
         <v>1009</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D50" s="13" t="s">
         <v>10</v>
@@ -3058,7 +3061,7 @@
         <v>14</v>
       </c>
       <c r="M50" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N50" s="11"/>
       <c r="O50" s="5"/>
@@ -3068,10 +3071,10 @@
         <v>51</v>
       </c>
       <c r="B51" s="61" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D51" s="13" t="s">
         <v>31</v>
@@ -3097,7 +3100,7 @@
         <v>14</v>
       </c>
       <c r="M51" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N51" s="11"/>
       <c r="O51" s="5"/>
@@ -3132,7 +3135,7 @@
         <v>36</v>
       </c>
       <c r="M52" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N52" s="11"/>
       <c r="O52" s="11"/>
@@ -3162,7 +3165,7 @@
       </c>
       <c r="I53" s="17"/>
       <c r="J53" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K53" s="17">
         <v>16</v>
@@ -3171,7 +3174,7 @@
         <v>36</v>
       </c>
       <c r="M53" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N53" s="11"/>
       <c r="O53" s="11"/>
@@ -3210,7 +3213,7 @@
         <v>14</v>
       </c>
       <c r="M54" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N54" s="11"/>
       <c r="O54" s="5"/>
@@ -3220,10 +3223,10 @@
         <v>51</v>
       </c>
       <c r="B55" s="61" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>31</v>
@@ -3249,7 +3252,7 @@
         <v>14</v>
       </c>
       <c r="M55" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="N55" s="11"/>
       <c r="O55" s="5"/>
@@ -3262,7 +3265,7 @@
         <v>3098</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>10</v>
@@ -3288,7 +3291,7 @@
         <v>14</v>
       </c>
       <c r="M56" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="N56" s="11"/>
       <c r="O56" s="5"/>
@@ -3298,10 +3301,10 @@
         <v>51</v>
       </c>
       <c r="B57" s="61" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D57" s="13" t="s">
         <v>31</v>
@@ -3327,7 +3330,7 @@
         <v>14</v>
       </c>
       <c r="M57" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="N57" s="11"/>
       <c r="O57" s="5"/>
@@ -3340,7 +3343,7 @@
         <v>3087</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D58" s="13" t="s">
         <v>10</v>
@@ -3366,7 +3369,7 @@
         <v>14</v>
       </c>
       <c r="M58" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="N58" s="34"/>
       <c r="O58" s="34"/>
@@ -3396,7 +3399,7 @@
       </c>
       <c r="I59" s="17"/>
       <c r="J59" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K59" s="17">
         <v>16</v>
@@ -3405,7 +3408,7 @@
         <v>36</v>
       </c>
       <c r="M59" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N59" s="34"/>
       <c r="O59" s="34"/>
@@ -3415,10 +3418,10 @@
         <v>53</v>
       </c>
       <c r="B60" s="33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D60" s="13" t="s">
         <v>31</v>
@@ -3444,7 +3447,7 @@
         <v>14</v>
       </c>
       <c r="M60" s="12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N60" s="12"/>
       <c r="O60" s="16"/>
@@ -3454,10 +3457,10 @@
         <v>51</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D61" s="13" t="s">
         <v>31</v>
@@ -3483,7 +3486,7 @@
         <v>14</v>
       </c>
       <c r="M61" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N61" s="12"/>
       <c r="O61" s="16"/>
@@ -3496,7 +3499,7 @@
         <v>4885</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D62" s="13" t="s">
         <v>10</v>
@@ -3522,7 +3525,7 @@
         <v>14</v>
       </c>
       <c r="M62" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N62" s="11"/>
       <c r="O62" s="11"/>

</xml_diff>